<commit_message>
Implementadas validaciones de la interfaz asi como el actualizar del tree y el reiniciar periodo
</commit_message>
<xml_diff>
--- a/app-RRHH/file/evaluacion.xlsx
+++ b/app-RRHH/file/evaluacion.xlsx
@@ -577,12 +577,12 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E198"/>
+  <dimension ref="A1:E253"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.40625" defaultRowHeight="21.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -634,2354 +634,3014 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DIRECCION</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MARITZA MOYA CUELLAR</t>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ARMINDA JULIA ARIAS  HERNÁNDEZ</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DIRECCION</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ARTURO EVASIO SÁNCHEZ  MARTÍNEZ</t>
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>CONSUELO GONZÁLEZ  DÍAZ</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>DIRECCION</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ERIK LÁZARO PRENDES LAGO</t>
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>LEONEL SILVA  ABAD</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>DIRECCION</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>DILENIA HIDALGO SUÁREZ</t>
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>YUNIERT CUTIÑO  GRIÑAN</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>DIRECCION</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ONEDIS BASULTO HERNÁNDEZ</t>
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>EDUARDO GONZÁLEZ  FERNÁNDEZ</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION COMERCIAL</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>CLAUDIA LINARES  SOSA</t>
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>IDARMIS RIVERA  LEÓN</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION COMERCIAL</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>EDGAR SÁNCHEZ  OLIVA</t>
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>PABLO PÉREZ  TORRES</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION COMERCIAL</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JANETT ADRIANA VÁZQUEZ  FANEGO</t>
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ESTEBAN DAVID SÁNCHEZ  NOVO</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION COMERCIAL</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ADRIANA VALERA CORREA</t>
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>JULIO ESTEBAN FIGUEREDO  DEL TORO</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SUILEN REYES  SUÁREZ</t>
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>MIGUEL ANGEL CÁRDENAS  FERNÁNDEZ</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ISIS IVETTE ESCALONA LEYVA</t>
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>DANCÉS LEÓN  HERRERA</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>TERESA DE LA CARIDAD GARCÍA  BOLAÑOS</t>
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>YUSNIEL MOJENA  CAMPILLO</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>JOSE LUIS CATURLA TERRY</t>
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>YOEL MONDUY  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>LEONARDO PEREZ RAMIREZ</t>
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>ELIEZER SENÉN MEDINA  CARBONELL</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>ERNESTO GUERRA MATA</t>
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ANA JULIA GONZÁLEZ GÓMEZ</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>CARLOS  DIAZ ORDAZ</t>
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>VIRGINIA ISABEL SOTO  CASTRO</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE DESARROLLO</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>RAÚL PAVÓN  FUENTES</t>
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>YAMILKA DE LA CARIDAD SOSA  REMÓN</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE DESARROLLO</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>DANAY GUZMÁN BORGES</t>
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>VALIA NOGUERA FIGUEROA</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE DESARROLLO</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>MARTHA BRENDA DÍAZ DELGADO</t>
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>SANDOR RUBÉN  ROLDÁN</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION INFORMATICA</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>FRANCISCO JAVIER CASTELLÓN  BARTROLI</t>
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ARIANNA GUZMÁN RIVERO</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION INFORMATICA</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>EDUARDO  FORTE MARQUEZ</t>
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>KENIA AMINTA DELGADO  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION INFORMATICA</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>ALEJANDRO  RAMÍREZ COMESAÑAS</t>
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ANAEVI MARTÍNEZ  RAMOS</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>YAMILA JO  MARRERO</t>
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ALAIN GARCÍA  JEREZ</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>ROBERTO PADILLA  COLAO</t>
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>MARIA DEL  CARMEN CASTAÑER  AVERHOFF</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>HASLEMER SOTOLONGO  CUZA</t>
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>RODOBALDO DÍAZ  ARTEAGA</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>REMBERTO GONZÁLEZ MORALES</t>
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>LUIS ANGEL GARCÍA ALARCÓN</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>GRUPO ALMACEN SIBONEY</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>HERMINIO LAGARZA  ACOSTA</t>
+      <c r="A29" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>BÁRBARO PABLO GONZÁLEZ  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>GRUPO ALMACEN SIBONEY</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>ERNESTO SÁNCHEZ  COLUMBIÉ</t>
+      <c r="A30" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ORLANDO LLANES  MESA</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>GRUPO ALMACEN SIBONEY</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>ALEJANDRO MONTAÑA  RIVERA</t>
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>JESUS BARCELONA  ALAMBARES</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>GRUPO ALMACEN SIBONEY</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>ROLANDO RODRIGUEZ GONZALEZ</t>
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>OSMEL DÍAZ  CRUZ</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>JULIO CÉSAR ESCAÑO  RODRÍGUEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ALAIN MERCHÁN  OLIVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>JORGE ALBERTO GOENAGA  MARTÍNEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>DENNIS ORTIZ  HERNÁNDEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>JULIO CESAR BERMUDEZ  LOPEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>YANOSKY ESCAÑO  RODRÍGUEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>RAYWER SIERRA  RODRÍGUEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>JONAH LÓPEZ  DÍAZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>YADIRA FERRARI  SUÁREZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>MAIKEL CÓRDOVA  GÓNGORA</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>OSMEL IGNACIO FERNÁNDEZ  CAMPILLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>LIVIO AVELINO LIMONTA JIMENEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>YAN LUIS MARTINEZ GONZALEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>MAXIMO MENDEZ MOLINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>ABEL ERNESTO URGELLES GARRIDO</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ARNALDO BLANCO  CARDOSO</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>OMAR VEGA  SIERRA</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ROBERTO AGUIRREZABAL  HOPUY</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>ARNALDO BLANCO  CARDOSO</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>MELVIN PADRÓN  FLEITAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>ROBERTO AGUIRREZABAL  HOPUY</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>LIOSBEL VALDÉS  HERRERA</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>LIOSBEL VALDÉS  HERRERA</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>JORGE LUIS MARTÍNEZ  GONZÁLEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>JORGE LUIS MARTÍNEZ  GONZÁLEZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t>REGINO MARRERO  TAMAYO</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>REGINO MARRERO  TAMAYO</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t>VLADIMIR  CLARO  NIKOLAIEVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>VLADIMIR  CLARO  NIKOLAIEVA</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>MANUEL GARCÍA  GUTIERREZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>MANUEL GARCÍA  GUTIERREZ</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t>ARMANDO ÁLVAREZ  FERNÁNDEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B56" s="0" t="inlineStr">
         <is>
           <t>JORGE PABLO RODRÍGUEZ  SÁNCHEZ</t>
         </is>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+    <row r="57">
+      <c r="A57" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B57" s="0" t="inlineStr">
         <is>
           <t>JORJAN OLIVERA  MONTANO</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="58">
+      <c r="A58" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B58" s="0" t="inlineStr">
         <is>
           <t>LÁZARO REINIER RODRÍGUEZ RAVELO</t>
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+    <row r="59">
+      <c r="A59" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t>LUIS ALBERTO PITA BODAÑO</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="inlineStr">
+        <is>
+          <t>SUBDIRECCION DE OPERACIONES</t>
+        </is>
+      </c>
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>MICHEL BARZAGA URQUIZA</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="inlineStr">
+        <is>
+          <t>SUBDIRECCION DE OPERACIONES</t>
+        </is>
+      </c>
+      <c r="B61" s="0" t="inlineStr">
         <is>
           <t>OSMAR MANUEL VAILLANT QUEZADA</t>
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+    <row r="62">
+      <c r="A62" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B62" s="0" t="inlineStr">
+        <is>
+          <t>OSMEL LEONARDO ZAMORA PEREZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="inlineStr">
+        <is>
+          <t>SUBDIRECCION DE OPERACIONES</t>
+        </is>
+      </c>
+      <c r="B63" s="0" t="inlineStr">
         <is>
           <t>YANSEL GONZALEZ VARELA</t>
         </is>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
+    <row r="64">
+      <c r="A64" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B64" s="0" t="inlineStr">
         <is>
           <t>DANIEL SANTIAGO RAMOS VALLS</t>
         </is>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
+    <row r="65">
+      <c r="A65" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B65" s="0" t="inlineStr">
         <is>
           <t>BENIGNO GONZALEZ ORTIZ</t>
         </is>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
+    <row r="66">
+      <c r="A66" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B66" s="0" t="inlineStr">
         <is>
           <t>ARIEL PEÑA  NAPOLES</t>
         </is>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+    <row r="67">
+      <c r="A67" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B67" s="0" t="inlineStr">
         <is>
           <t>DIMAS MARCOS IBALBIA PAIROL</t>
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
+    <row r="68">
+      <c r="A68" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B68" s="0" t="inlineStr">
+        <is>
+          <t>ALEXEI BERNIS VILTRES</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="inlineStr">
+        <is>
+          <t>SUBDIRECCION DE OPERACIONES</t>
+        </is>
+      </c>
+      <c r="B69" s="0" t="inlineStr">
         <is>
           <t>EMIGDIO JIMÉNEZ PEÑA</t>
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
+    <row r="70">
+      <c r="A70" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B70" s="0" t="inlineStr">
         <is>
           <t>JUAN ALEXANDER  ALBUQUERQUE HERRERA</t>
         </is>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
+    <row r="71">
+      <c r="A71" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B71" s="0" t="inlineStr">
         <is>
           <t>NOEL FERNÁNDEZ VARELA</t>
         </is>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+    <row r="72">
+      <c r="A72" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION TECNICA</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B72" s="0" t="inlineStr">
+        <is>
+          <t>FLORENTINO FERNÁNDEZ  MOLINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0" t="inlineStr">
+        <is>
+          <t>SUBDIRECCION TECNICA</t>
+        </is>
+      </c>
+      <c r="B73" s="0" t="inlineStr">
         <is>
           <t>YEAN MARC MORENO  CABRERA</t>
         </is>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
+    <row r="74">
+      <c r="A74" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION TECNICA</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B74" s="0" t="inlineStr">
         <is>
           <t>ISRAEL MORA  BELTRÁN</t>
         </is>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+    <row r="75">
+      <c r="A75" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION TECNICA</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B75" s="0" t="inlineStr">
         <is>
           <t>RAMÓN OQUENDO  FADRAGA</t>
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
+    <row r="76">
+      <c r="A76" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION TECNICA</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B76" s="0" t="inlineStr">
         <is>
           <t>ALFREDO VAGNER PEÑA SILVA</t>
         </is>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
+    <row r="77">
+      <c r="A77" s="0" t="inlineStr">
         <is>
           <t>SUBDIRECCION TECNICA</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B77" s="0" t="inlineStr">
         <is>
           <t>JUAN CARLOS YAMACHO SILVA</t>
         </is>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
+    <row r="78">
+      <c r="A78" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="B78" s="0" t="inlineStr">
+        <is>
+          <t>ANGEL DANIEL PASCUAL  VALDÉS</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER BOYEROS</t>
+        </is>
+      </c>
+      <c r="B79" s="0" t="inlineStr">
+        <is>
+          <t>HENRY ROLANDO ESTEVEZ  CALDERÓN</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER BOYEROS</t>
+        </is>
+      </c>
+      <c r="B80" s="0" t="inlineStr">
         <is>
           <t>ALEJANDRO BATISTA  CRUZ</t>
         </is>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
+    <row r="81">
+      <c r="A81" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B81" s="0" t="inlineStr">
         <is>
           <t>DANIEL ALEJANDRO JIMENEZ BETANCOURT</t>
         </is>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
+    <row r="82">
+      <c r="A82" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="B82" s="0" t="inlineStr">
         <is>
           <t>ALDO  OLIVEROS  CRUZ</t>
         </is>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
+    <row r="83">
+      <c r="A83" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B83" s="0" t="inlineStr">
         <is>
           <t>IVAN  CRUZ GARCIA</t>
         </is>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
+    <row r="84">
+      <c r="A84" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B84" s="0" t="inlineStr">
         <is>
           <t>EDDY RODRÍGUEZ CARBALLEDO</t>
         </is>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
+    <row r="85">
+      <c r="A85" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER BOYEROS</t>
+        </is>
+      </c>
+      <c r="B85" s="0" t="inlineStr">
+        <is>
+          <t>REINIER ESTRADA VIVES</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER BOYEROS</t>
+        </is>
+      </c>
+      <c r="B86" s="0" t="inlineStr">
+        <is>
+          <t>JOAQUIN MODESTO PERDOMO PEREZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER HABANA</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B87" s="0" t="inlineStr">
+        <is>
+          <t>IBRAHIN FERRER  DE LA ROSA</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER HABANA</t>
+        </is>
+      </c>
+      <c r="B88" s="0" t="inlineStr">
         <is>
           <t>MIGUEL VALLE  ÁLVAREZ</t>
         </is>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
+    <row r="89">
+      <c r="A89" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER HABANA</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B89" s="0" t="inlineStr">
         <is>
           <t>WILLIAN RODRÍGUEZ VELIZ</t>
         </is>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
+    <row r="90">
+      <c r="A90" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER HABANA</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B90" s="0" t="inlineStr">
         <is>
           <t>JUAN DE LEÓN  CARMENATY</t>
         </is>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
+    <row r="91">
+      <c r="A91" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="B91" s="0" t="inlineStr">
+        <is>
+          <t>REINALDO RAMOS  GÓMEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B92" s="0" t="inlineStr">
         <is>
           <t>JORGE LUIS LÓPEZ  ORTA</t>
         </is>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
+    <row r="93">
+      <c r="A93" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B93" s="0" t="inlineStr">
         <is>
           <t>YANET DEVESA  SÁNCHEZ</t>
         </is>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
+    <row r="94">
+      <c r="A94" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B94" s="0" t="inlineStr">
         <is>
           <t>ROBERTO FRANCISCO JARDÓN  PRENDES</t>
         </is>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
+    <row r="95">
+      <c r="A95" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B95" s="0" t="inlineStr">
         <is>
           <t>LEONARDO RODRÍGUEZ  MEDINA</t>
         </is>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
+    <row r="96">
+      <c r="A96" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B96" s="0" t="inlineStr">
+        <is>
+          <t>ERNESTO MELIAN  RODRÍGUEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B97" s="0" t="inlineStr">
+        <is>
+          <t>MOISES RICARDO VALDÉS  BELLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B98" s="0" t="inlineStr">
         <is>
           <t>ERNESTO ALARCÓN  ESPINOSA</t>
         </is>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
+    <row r="99">
+      <c r="A99" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B99" s="0" t="inlineStr">
         <is>
           <t>HUMBERTO PABLO CABEZAS   ALONSO</t>
         </is>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
+    <row r="100">
+      <c r="A100" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B100" s="0" t="inlineStr">
         <is>
           <t>LUIS DANIEL GONZÁLEZ  VIERA</t>
         </is>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
+    <row r="101">
+      <c r="A101" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B101" s="0" t="inlineStr">
+        <is>
+          <t>YORGENIS RAMÍREZ  VELÁZQUEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B102" s="0" t="inlineStr">
+        <is>
+          <t>JUAN CARLOS TRELLES  CABRERA</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B103" s="0" t="inlineStr">
         <is>
           <t>LUIS BULNES  CARRILLO</t>
         </is>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
+    <row r="104">
+      <c r="A104" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="B104" s="0" t="inlineStr">
         <is>
           <t>RICARDO DANIEL PÉREZ  ALLISON</t>
         </is>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
+    <row r="105">
+      <c r="A105" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B105" s="0" t="inlineStr">
         <is>
           <t>MALKIEL  MOJENA HERNANDEZ</t>
         </is>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
+    <row r="106">
+      <c r="A106" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B106" s="0" t="inlineStr">
         <is>
           <t>RAIDEL RAMOS ARREBATO</t>
         </is>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
+    <row r="107">
+      <c r="A107" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B107" s="0" t="inlineStr">
         <is>
           <t>ANTUAN UMPIERRE ALVAREZ</t>
         </is>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
+    <row r="108">
+      <c r="A108" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B108" s="0" t="inlineStr">
         <is>
           <t>ERANDIS  ALVAREZ GARCIA</t>
         </is>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
+    <row r="109">
+      <c r="A109" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="B109" s="0" t="inlineStr">
+        <is>
+          <t>LAZARO YORDAN VALDES BRUNET</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B110" s="0" t="inlineStr">
+        <is>
+          <t>YASER RENE LOPEZ BLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B111" s="0" t="inlineStr">
+        <is>
+          <t>CARLOS WILFREDO AROZARENA CORTES</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B112" s="0" t="inlineStr">
         <is>
           <t>ARMANDO LOPEZ GUERRA</t>
         </is>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
+    <row r="113">
+      <c r="A113" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B113" s="0" t="inlineStr">
         <is>
           <t>JEIBEL ALONSO SARDIÑAS</t>
         </is>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
+    <row r="114">
+      <c r="A114" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B114" s="0" t="inlineStr">
+        <is>
+          <t>JOSE LUIS MÁRQUEZ VICO</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B115" s="0" t="inlineStr">
+        <is>
+          <t>FRANKLIN ISMAEL PÉREZ ROMEU</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B116" s="0" t="inlineStr">
+        <is>
+          <t>YOESLAN  VALDES SANCHEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B117" s="0" t="inlineStr">
         <is>
           <t>DANIEL MUÑOZ GONZÁLEZ</t>
         </is>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
+    <row r="118">
+      <c r="A118" s="0" t="inlineStr">
         <is>
           <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B118" s="0" t="inlineStr">
         <is>
           <t>YASSER BOTELLO VIDAL</t>
         </is>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
+    <row r="119">
+      <c r="A119" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO TALLER SIBONEY</t>
+        </is>
+      </c>
+      <c r="B119" s="0" t="inlineStr">
+        <is>
+          <t>YURY ROBERTO CONYEDO ALEJO</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B120" s="0" t="inlineStr">
         <is>
           <t>ARMINDA JULIA ARIAS  HERNÁNDEZ</t>
         </is>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
+    <row r="121">
+      <c r="A121" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B121" s="0" t="inlineStr">
         <is>
           <t>CONSUELO GONZÁLEZ  DÍAZ</t>
         </is>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
+    <row r="122">
+      <c r="A122" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B122" s="0" t="inlineStr">
         <is>
           <t>LEONEL SILVA  ABAD</t>
         </is>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
+    <row r="123">
+      <c r="A123" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B123" s="0" t="inlineStr">
         <is>
           <t>YUNIERT CUTIÑO  GRIÑAN</t>
         </is>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
+    <row r="124">
+      <c r="A124" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B124" s="0" t="inlineStr">
+        <is>
+          <t>EDUARDO GONZÁLEZ  FERNÁNDEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B125" s="0" t="inlineStr">
         <is>
           <t>IDARMIS RIVERA  LEÓN</t>
         </is>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
+    <row r="126">
+      <c r="A126" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B126" s="0" t="inlineStr">
+        <is>
+          <t>PABLO PÉREZ  TORRES</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B127" s="0" t="inlineStr">
         <is>
           <t>ESTEBAN DAVID SÁNCHEZ  NOVO</t>
         </is>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
+    <row r="128">
+      <c r="A128" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B128" s="0" t="inlineStr">
         <is>
           <t>JULIO ESTEBAN FIGUEREDO  DEL TORO</t>
         </is>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
+    <row r="129">
+      <c r="A129" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B129" s="0" t="inlineStr">
         <is>
           <t>MIGUEL ANGEL CÁRDENAS  FERNÁNDEZ</t>
         </is>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
+    <row r="130">
+      <c r="A130" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B130" s="0" t="inlineStr">
         <is>
           <t>DANCÉS LEÓN  HERRERA</t>
         </is>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
+    <row r="131">
+      <c r="A131" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B131" s="0" t="inlineStr">
         <is>
           <t>YUSNIEL MOJENA  CAMPILLO</t>
         </is>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
+    <row r="132">
+      <c r="A132" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B132" s="0" t="inlineStr">
         <is>
           <t>YOEL MONDUY  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
+    <row r="133">
+      <c r="A133" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B133" s="0" t="inlineStr">
         <is>
           <t>ELIEZER SENÉN MEDINA  CARBONELL</t>
         </is>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
+    <row r="134">
+      <c r="A134" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B134" s="0" t="inlineStr">
         <is>
           <t>ANA JULIA GONZÁLEZ GÓMEZ</t>
         </is>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
+    <row r="135">
+      <c r="A135" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B135" s="0" t="inlineStr">
         <is>
           <t>VIRGINIA ISABEL SOTO  CASTRO</t>
         </is>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
+    <row r="136">
+      <c r="A136" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B136" s="0" t="inlineStr">
         <is>
           <t>YAMILKA DE LA CARIDAD SOSA  REMÓN</t>
         </is>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
+    <row r="137">
+      <c r="A137" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B137" s="0" t="inlineStr">
         <is>
           <t>VALIA NOGUERA FIGUEROA</t>
         </is>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
+    <row r="138">
+      <c r="A138" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B138" s="0" t="inlineStr">
         <is>
           <t>SANDOR RUBÉN  ROLDÁN</t>
         </is>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
+    <row r="139">
+      <c r="A139" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B139" s="0" t="inlineStr">
         <is>
           <t>ARIANNA GUZMÁN RIVERO</t>
         </is>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
+    <row r="140">
+      <c r="A140" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B140" s="0" t="inlineStr">
         <is>
           <t>KENIA AMINTA DELGADO  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
+    <row r="141">
+      <c r="A141" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B141" s="0" t="inlineStr">
         <is>
           <t>ANAEVI MARTÍNEZ  RAMOS</t>
         </is>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
+    <row r="142">
+      <c r="A142" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B142" s="0" t="inlineStr">
         <is>
           <t>ALAIN GARCÍA  JEREZ</t>
         </is>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
+    <row r="143">
+      <c r="A143" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B143" s="0" t="inlineStr">
         <is>
           <t>MARIA DEL  CARMEN CASTAÑER  AVERHOFF</t>
         </is>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
+    <row r="144">
+      <c r="A144" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B144" s="0" t="inlineStr">
+        <is>
+          <t>RODOBALDO DÍAZ  ARTEAGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B145" s="0" t="inlineStr">
         <is>
           <t>LUIS ANGEL GARCÍA ALARCÓN</t>
         </is>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
+    <row r="146">
+      <c r="A146" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B146" s="0" t="inlineStr">
         <is>
           <t>BÁRBARO PABLO GONZÁLEZ  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
+    <row r="147">
+      <c r="A147" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B147" s="0" t="inlineStr">
         <is>
           <t>ORLANDO LLANES  MESA</t>
         </is>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
+    <row r="148">
+      <c r="A148" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B148" s="0" t="inlineStr">
         <is>
           <t>JESUS BARCELONA  ALAMBARES</t>
         </is>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
+    <row r="149">
+      <c r="A149" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B149" s="0" t="inlineStr">
         <is>
           <t>OSMEL DÍAZ  CRUZ</t>
         </is>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
+    <row r="150">
+      <c r="A150" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B150" s="0" t="inlineStr">
         <is>
           <t>JULIO CÉSAR ESCAÑO  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
+    <row r="151">
+      <c r="A151" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B151" s="0" t="inlineStr">
         <is>
           <t>ALAIN MERCHÁN  OLIVA</t>
         </is>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
+    <row r="152">
+      <c r="A152" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B152" s="0" t="inlineStr">
         <is>
           <t>JORGE ALBERTO GOENAGA  MARTÍNEZ</t>
         </is>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
+    <row r="153">
+      <c r="A153" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B153" s="0" t="inlineStr">
         <is>
           <t>DENNIS ORTIZ  HERNÁNDEZ</t>
         </is>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
+    <row r="154">
+      <c r="A154" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B154" s="0" t="inlineStr">
         <is>
           <t>JULIO CESAR BERMUDEZ  LOPEZ</t>
         </is>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
+    <row r="155">
+      <c r="A155" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B155" s="0" t="inlineStr">
         <is>
           <t>YANOSKY ESCAÑO  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
+    <row r="156">
+      <c r="A156" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B156" s="0" t="inlineStr">
         <is>
           <t>RAYWER SIERRA  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
+    <row r="157">
+      <c r="A157" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B157" s="0" t="inlineStr">
         <is>
           <t>JONAH LÓPEZ  DÍAZ</t>
         </is>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
+    <row r="158">
+      <c r="A158" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B158" s="0" t="inlineStr">
         <is>
           <t>YADIRA FERRARI  SUÁREZ</t>
         </is>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
+    <row r="159">
+      <c r="A159" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B159" s="0" t="inlineStr">
         <is>
           <t>MAIKEL CÓRDOVA  GÓNGORA</t>
         </is>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
+    <row r="160">
+      <c r="A160" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B160" s="0" t="inlineStr">
         <is>
           <t>OSMEL IGNACIO FERNÁNDEZ  CAMPILLO</t>
         </is>
       </c>
     </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
+    <row r="161">
+      <c r="A161" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B161" s="0" t="inlineStr">
         <is>
           <t>LIVIO AVELINO LIMONTA JIMENEZ</t>
         </is>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
+    <row r="162">
+      <c r="A162" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B162" s="0" t="inlineStr">
         <is>
           <t>YAN LUIS MARTINEZ GONZALEZ</t>
         </is>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
+    <row r="163">
+      <c r="A163" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO AEROPUERTO</t>
+        </is>
+      </c>
+      <c r="B163" s="0" t="inlineStr">
         <is>
           <t>MAXIMO MENDEZ MOLINA</t>
         </is>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
+    <row r="164">
+      <c r="A164" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE VENTAS PINAR DEL RIO</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr">
+      <c r="B164" s="0" t="inlineStr">
         <is>
           <t>LUIS MANUEL PUENTES  CID</t>
         </is>
       </c>
     </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
+    <row r="165">
+      <c r="A165" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE VENTAS PINAR DEL RIO</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr">
+      <c r="B165" s="0" t="inlineStr">
         <is>
           <t>FRANCISCO PALACIOS CABRERA</t>
         </is>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
+    <row r="166">
+      <c r="A166" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE VENTAS PINAR DEL RIO</t>
         </is>
       </c>
-      <c r="B127" t="inlineStr">
+      <c r="B166" s="0" t="inlineStr">
         <is>
           <t>PEDRO BEC LÓPEZ</t>
         </is>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
+    <row r="167">
+      <c r="A167" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE VENTAS PINAR DEL RIO</t>
         </is>
       </c>
-      <c r="B128" t="inlineStr">
+      <c r="B167" s="0" t="inlineStr">
         <is>
           <t>ADOLFO DAMIÁN MORENO GONZÁLEZ</t>
         </is>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
+    <row r="168">
+      <c r="A168" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B129" t="inlineStr">
+      <c r="B168" s="0" t="inlineStr">
         <is>
           <t>YOASMIN CALDERON  PÉREZ</t>
         </is>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
+    <row r="169">
+      <c r="A169" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr">
+      <c r="B169" s="0" t="inlineStr">
         <is>
           <t>AVELARDO IZQUIERDO  REYES</t>
         </is>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
+    <row r="170">
+      <c r="A170" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
+      <c r="B170" s="0" t="inlineStr">
         <is>
           <t>MANUEL RAÚL GÓMEZ  FERRO</t>
         </is>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
+    <row r="171">
+      <c r="A171" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr">
+      <c r="B171" s="0" t="inlineStr">
         <is>
           <t>PEDRO EMILIO CARNOT  PEREIRA</t>
         </is>
       </c>
     </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
+    <row r="172">
+      <c r="A172" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
+      <c r="B172" s="0" t="inlineStr">
         <is>
           <t>YUDITH REMIS  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
+    <row r="173">
+      <c r="A173" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
+      <c r="B173" s="0" t="inlineStr">
         <is>
           <t>ALEXIS SUÁREZ  CAPOTE</t>
         </is>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
+    <row r="174">
+      <c r="A174" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
+      <c r="B174" s="0" t="inlineStr">
+        <is>
+          <t>ENID CRESPO  TORRES</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO CIUDAD</t>
+        </is>
+      </c>
+      <c r="B175" s="0" t="inlineStr">
         <is>
           <t>OSVALDO MORENO  HERNÁNDEZ</t>
         </is>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
+    <row r="176">
+      <c r="A176" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr">
+      <c r="B176" s="0" t="inlineStr">
         <is>
           <t>DARIEL ORTIZ VALDEZ</t>
         </is>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
+    <row r="177">
+      <c r="A177" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
+      <c r="B177" s="0" t="inlineStr">
+        <is>
+          <t>JULIO GERMÁN MORA NEGRÍN</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO CIUDAD</t>
+        </is>
+      </c>
+      <c r="B178" s="0" t="inlineStr">
         <is>
           <t>ISEL ENAMORADO ODUARDO</t>
         </is>
       </c>
     </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
+    <row r="179">
+      <c r="A179" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
+      <c r="B179" s="0" t="inlineStr">
         <is>
           <t>ALFREDO LOPEZ ALEMAN</t>
         </is>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
+    <row r="180">
+      <c r="A180" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
+      <c r="B180" s="0" t="inlineStr">
         <is>
           <t>DIOSDADO VIZCAINO  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
+    <row r="181">
+      <c r="A181" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
+      <c r="B181" s="0" t="inlineStr">
         <is>
           <t>MARIANELA MANCHA TARAJANO</t>
         </is>
       </c>
     </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
+    <row r="182">
+      <c r="A182" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
+      <c r="B182" s="0" t="inlineStr">
+        <is>
+          <t>MAILYN LORENZO  RODRÍGUEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO VARADERO</t>
+        </is>
+      </c>
+      <c r="B183" s="0" t="inlineStr">
         <is>
           <t>YUDIETH PALENZUELA  YANES</t>
         </is>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
+    <row r="184">
+      <c r="A184" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr">
+      <c r="B184" s="0" t="inlineStr">
         <is>
           <t>SHEYLA NORES  GONZÁLEZ</t>
         </is>
       </c>
     </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
+    <row r="185">
+      <c r="A185" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B143" t="inlineStr">
+      <c r="B185" s="0" t="inlineStr">
         <is>
           <t>JAVIEL PITA  CABALLERO</t>
         </is>
       </c>
     </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
+    <row r="186">
+      <c r="A186" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr">
+      <c r="B186" s="0" t="inlineStr">
         <is>
           <t>MICHAEL DE ARMAS  RODRÍGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
+    <row r="187">
+      <c r="A187" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr">
+      <c r="B187" s="0" t="inlineStr">
         <is>
           <t>ARTURO DÁVALOS  MOROS</t>
         </is>
       </c>
     </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
+    <row r="188">
+      <c r="A188" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B146" t="inlineStr">
+      <c r="B188" s="0" t="inlineStr">
         <is>
           <t>JOAQUÍN FERNÁNDEZ  RONDÓN</t>
         </is>
       </c>
     </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
+    <row r="189">
+      <c r="A189" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
-      <c r="B147" t="inlineStr">
+      <c r="B189" s="0" t="inlineStr">
         <is>
           <t>LUIS ANTONIO NARANJO  QUINTANA</t>
         </is>
       </c>
     </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
+    <row r="190">
+      <c r="A190" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO VARADERO</t>
+        </is>
+      </c>
+      <c r="B190" s="0" t="inlineStr">
+        <is>
+          <t>YOAN  HERNÁNDEZ  MENDEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
+      <c r="B191" s="0" t="inlineStr">
         <is>
           <t>FÉLIX MEDINA  SUÁREZ</t>
         </is>
       </c>
     </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
+    <row r="192">
+      <c r="A192" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
+      <c r="B192" s="0" t="inlineStr">
         <is>
           <t>ANA MARIA HERNÁNDEZ  GONZÁLEZ</t>
         </is>
       </c>
     </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
+    <row r="193">
+      <c r="A193" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
+      <c r="B193" s="0" t="inlineStr">
         <is>
           <t>EDEL JIMÉNEZ  ALBA</t>
         </is>
       </c>
     </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
+    <row r="194">
+      <c r="A194" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B151" t="inlineStr">
+      <c r="B194" s="0" t="inlineStr">
         <is>
           <t>ALBERTO PÉREZ  FLORES</t>
         </is>
       </c>
     </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
+    <row r="195">
+      <c r="A195" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B152" t="inlineStr">
+      <c r="B195" s="0" t="inlineStr">
         <is>
           <t>CARLOS ENRIQUE VELASCO  BLANCO</t>
         </is>
       </c>
     </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
+    <row r="196">
+      <c r="A196" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B153" t="inlineStr">
+      <c r="B196" s="0" t="inlineStr">
+        <is>
+          <t>PABLO GARCÍA MARTÍNEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO VILLA CLARA</t>
+        </is>
+      </c>
+      <c r="B197" s="0" t="inlineStr">
         <is>
           <t>EVIS ACUÑA BRAVO</t>
         </is>
       </c>
     </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
+    <row r="198">
+      <c r="A198" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
+      <c r="B198" s="0" t="inlineStr">
         <is>
           <t>FAUSTINO RODRIGUEZ RODRIGUEZ</t>
         </is>
       </c>
     </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
+    <row r="199">
+      <c r="A199" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B155" t="inlineStr">
+      <c r="B199" s="0" t="inlineStr">
         <is>
           <t>RAUL  RODRIGUEZ SANCHEZ</t>
         </is>
       </c>
     </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
+    <row r="200">
+      <c r="A200" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B156" t="inlineStr">
+      <c r="B200" s="0" t="inlineStr">
         <is>
           <t>FRANK NIEBLA BERMUDEZ</t>
         </is>
       </c>
     </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
+    <row r="201">
+      <c r="A201" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B157" t="inlineStr">
+      <c r="B201" s="0" t="inlineStr">
         <is>
           <t>VLADIMIR  MANSO GONZÁLEZ</t>
         </is>
       </c>
     </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
+    <row r="202">
+      <c r="A202" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr">
+      <c r="B202" s="0" t="inlineStr">
         <is>
           <t>YOSVANY ECHEVARRÍA TURIÑO</t>
         </is>
       </c>
     </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
+    <row r="203">
+      <c r="A203" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr">
+      <c r="B203" s="0" t="inlineStr">
         <is>
           <t>LUIS MIGUEL MOYA PEREZ</t>
         </is>
       </c>
     </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
+    <row r="204">
+      <c r="A204" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
-      <c r="B160" t="inlineStr">
+      <c r="B204" s="0" t="inlineStr">
         <is>
           <t>ALFONSO COLINA  HURTADO</t>
         </is>
       </c>
     </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
+    <row r="205">
+      <c r="A205" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr">
+      <c r="B205" s="0" t="inlineStr">
         <is>
           <t>LUIS ORLANDO MARTIN  MAYONADA</t>
         </is>
       </c>
     </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
+    <row r="206">
+      <c r="A206" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
-      <c r="B162" t="inlineStr">
+      <c r="B206" s="0" t="inlineStr">
         <is>
           <t>MIRTA CABRERA GINORIA</t>
         </is>
       </c>
     </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
+    <row r="207">
+      <c r="A207" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
-      <c r="B163" t="inlineStr">
+      <c r="B207" s="0" t="inlineStr">
         <is>
           <t>ROLANDO GÓMEZ  SERRANO</t>
         </is>
       </c>
     </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
+    <row r="208">
+      <c r="A208" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
-      <c r="B164" t="inlineStr">
+      <c r="B208" s="0" t="inlineStr">
+        <is>
+          <t>LUIS ANGEL YERA PEREZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO CIENFUEGOS</t>
+        </is>
+      </c>
+      <c r="B209" s="0" t="inlineStr">
         <is>
           <t>ADEL  FERNANDEZ GONZALEZ</t>
         </is>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
+    <row r="210">
+      <c r="A210" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
-      <c r="B165" t="inlineStr">
+      <c r="B210" s="0" t="inlineStr">
         <is>
           <t>JESUS RAFAEL  DELGADO GESSA</t>
         </is>
       </c>
     </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
+    <row r="211">
+      <c r="A211" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
-      <c r="B166" t="inlineStr">
+      <c r="B211" s="0" t="inlineStr">
+        <is>
+          <t>JUAN CARLOS ABDALA  GARCÍA</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+        </is>
+      </c>
+      <c r="B212" s="0" t="inlineStr">
         <is>
           <t>ABUNDIO MOYA  PÉREZ</t>
         </is>
       </c>
     </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
+    <row r="213">
+      <c r="A213" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
+      <c r="B213" s="0" t="inlineStr">
+        <is>
+          <t>MARTINIANO HERNÁNDEZ  BARCELÓ</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+        </is>
+      </c>
+      <c r="B214" s="0" t="inlineStr">
+        <is>
+          <t>ALYS GARCÍA  HERNÁNDEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+        </is>
+      </c>
+      <c r="B215" s="0" t="inlineStr">
         <is>
           <t>GEORLANDY  VENEGA SANTOS</t>
         </is>
       </c>
     </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
+    <row r="216">
+      <c r="A216" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
-      <c r="B168" t="inlineStr">
+      <c r="B216" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">JOSE CARLOS  SANCHEZ  CID </t>
         </is>
       </c>
     </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
+    <row r="217">
+      <c r="A217" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
-      <c r="B169" t="inlineStr">
+      <c r="B217" s="0" t="inlineStr">
         <is>
           <t>ADRIÁN RODRÍGUEZ BARRERAS</t>
         </is>
       </c>
     </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
+    <row r="218">
+      <c r="A218" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
-      <c r="B170" t="inlineStr">
+      <c r="B218" s="0" t="inlineStr">
+        <is>
+          <t>ERIBERTO RAÚL VALDÉS  FONTELA</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO CAMAGUEY</t>
+        </is>
+      </c>
+      <c r="B219" s="0" t="inlineStr">
         <is>
           <t>PATRICIO HERNÁNDEZ  FÁBREGAS</t>
         </is>
       </c>
     </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
+    <row r="220">
+      <c r="A220" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
-      <c r="B171" t="inlineStr">
+      <c r="B220" s="0" t="inlineStr">
         <is>
           <t>ALEXIS ELIA CASTILLO  JIMÉNEZ</t>
         </is>
       </c>
     </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
+    <row r="221">
+      <c r="A221" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
+      <c r="B221" s="0" t="inlineStr">
         <is>
           <t>DUANY RICHARD VIGO MARRERO</t>
         </is>
       </c>
     </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
+    <row r="222">
+      <c r="A222" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
+      <c r="B222" s="0" t="inlineStr">
         <is>
           <t>HECTOR EUTIQUIO MOYARES  RAMOS</t>
         </is>
       </c>
     </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
+    <row r="223">
+      <c r="A223" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
+      <c r="B223" s="0" t="inlineStr">
         <is>
           <t>FERNANDO RODRÍGUEZ  CRUZ</t>
         </is>
       </c>
     </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
+    <row r="224">
+      <c r="A224" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B175" t="inlineStr">
+      <c r="B224" s="0" t="inlineStr">
         <is>
           <t>LIDISMIR DOROTEA VEGA  ARENA</t>
         </is>
       </c>
     </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
+    <row r="225">
+      <c r="A225" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
+      <c r="B225" s="0" t="inlineStr">
         <is>
           <t>LUIS ROBERTO ALMAGUER  SOLIS</t>
         </is>
       </c>
     </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
+    <row r="226">
+      <c r="A226" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
+      <c r="B226" s="0" t="inlineStr">
+        <is>
+          <t>NESTOR ERITH HERNÁNDEZ  MENA</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO HOLGUIN</t>
+        </is>
+      </c>
+      <c r="B227" s="0" t="inlineStr">
         <is>
           <t>RAMÓN SALINA  RICARDO</t>
         </is>
       </c>
     </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
+    <row r="228">
+      <c r="A228" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B178" t="inlineStr">
+      <c r="B228" s="0" t="inlineStr">
         <is>
           <t>YOSVANY PRIETO  MERIÑO</t>
         </is>
       </c>
     </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
+    <row r="229">
+      <c r="A229" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B179" t="inlineStr">
+      <c r="B229" s="0" t="inlineStr">
         <is>
           <t>JORGE LUIS SAAVEDRA  GARCÍA</t>
         </is>
       </c>
     </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
+    <row r="230">
+      <c r="A230" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr">
+      <c r="B230" s="0" t="inlineStr">
+        <is>
+          <t>ANNIER  CHAVEZ  LECTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO HOLGUIN</t>
+        </is>
+      </c>
+      <c r="B231" s="0" t="inlineStr">
         <is>
           <t>ROBERQUI HECHAVARRIA ALBA</t>
         </is>
       </c>
     </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
+    <row r="232">
+      <c r="A232" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B181" t="inlineStr">
+      <c r="B232" s="0" t="inlineStr">
         <is>
           <t>SERGIO YANSEL SARMIENTO CRUZ</t>
         </is>
       </c>
     </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
+    <row r="233">
+      <c r="A233" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr">
+      <c r="B233" s="0" t="inlineStr">
+        <is>
+          <t>CARLOS COBIRLLA AGUILERA</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="0" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO HOLGUIN</t>
+        </is>
+      </c>
+      <c r="B234" s="0" t="inlineStr">
         <is>
           <t>OSMANIS FERNANDEZ ANZARDO</t>
         </is>
       </c>
     </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
+    <row r="235">
+      <c r="A235" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr">
+      <c r="B235" s="0" t="inlineStr">
         <is>
           <t>ALEXIS RODRÍGUEZ CARRALERO</t>
         </is>
       </c>
     </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
+    <row r="236">
+      <c r="A236" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B184" t="inlineStr">
+      <c r="B236" s="0" t="inlineStr">
         <is>
           <t>ALFREDO IGARZA  BARRIEL</t>
         </is>
       </c>
     </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
+    <row r="237">
+      <c r="A237" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B185" t="inlineStr">
+      <c r="B237" s="0" t="inlineStr">
         <is>
           <t>JOSE ALAIN MASSO  ALMENARES</t>
         </is>
       </c>
     </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
+    <row r="238">
+      <c r="A238" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B186" t="inlineStr">
+      <c r="B238" s="0" t="inlineStr">
         <is>
           <t>ILIAT REVILLA  BARRIENTOS</t>
         </is>
       </c>
     </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
+    <row r="239">
+      <c r="A239" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
+      <c r="B239" s="0" t="inlineStr">
         <is>
           <t>DIUNEIKY GIRÓN  NOA</t>
         </is>
       </c>
     </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
+    <row r="240">
+      <c r="A240" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B188" t="inlineStr">
+      <c r="B240" s="0" t="inlineStr">
         <is>
           <t>ALEXANDER MARTÍNEZ  VIDAL</t>
         </is>
       </c>
     </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
+    <row r="241">
+      <c r="A241" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B189" t="inlineStr">
+      <c r="B241" s="0" t="inlineStr">
         <is>
           <t>ALFREDO RODRÍGUEZ  LEÓN</t>
         </is>
       </c>
     </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
+    <row r="242">
+      <c r="A242" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B190" t="inlineStr">
+      <c r="B242" s="0" t="inlineStr">
         <is>
           <t>GRISEL ORTEGA  ALVAREZ</t>
         </is>
       </c>
     </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
+    <row r="243">
+      <c r="A243" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B191" t="inlineStr">
+      <c r="B243" s="0" t="inlineStr">
         <is>
           <t>LEYANNE MEDINA  SANABIA</t>
         </is>
       </c>
     </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
+    <row r="244">
+      <c r="A244" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr">
+      <c r="B244" s="0" t="inlineStr">
         <is>
           <t>YOELKIS VIAMONTE  MENDOZA</t>
         </is>
       </c>
     </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
+    <row r="245">
+      <c r="A245" s="0" t="inlineStr">
         <is>
           <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr">
+      <c r="B245" s="0" t="inlineStr">
         <is>
           <t>ARNULFO EDGAR LUNA  MENDOZA</t>
         </is>
       </c>
     </row>
-    <row r="194">
-      <c r="A194" t="inlineStr">
+    <row r="246">
+      <c r="A246" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE SEGURIDAD INTERNA</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr">
+      <c r="B246" s="0" t="inlineStr">
         <is>
           <t>ROBERTO SUÁREZ  ANTÚNEZ</t>
         </is>
       </c>
     </row>
-    <row r="195">
-      <c r="A195" t="inlineStr">
+    <row r="247">
+      <c r="A247" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE SEGURIDAD INTERNA</t>
         </is>
       </c>
-      <c r="B195" t="inlineStr">
+      <c r="B247" s="0" t="inlineStr">
         <is>
           <t>FRANCISCO JIMÉNEZ  FÚ</t>
         </is>
       </c>
     </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
+    <row r="248">
+      <c r="A248" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE SEGURIDAD INTERNA</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
+      <c r="B248" s="0" t="inlineStr">
         <is>
           <t>ROLANDO  GONZALEZ PADRO</t>
         </is>
       </c>
     </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
+    <row r="249">
+      <c r="A249" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE SEGURIDAD INTERNA</t>
         </is>
       </c>
-      <c r="B197" t="inlineStr">
+      <c r="B249" s="0" t="inlineStr">
         <is>
           <t>HECTOR DANIEL MENDOZA VAZQUEZ</t>
         </is>
       </c>
     </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
+    <row r="250">
+      <c r="A250" s="0" t="inlineStr">
         <is>
           <t>GRUPO DE SEGURIDAD INTERNA</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr">
+      <c r="B250" s="0" t="inlineStr">
+        <is>
+          <t>ANDY  FERNANDEZ RAMON</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO DE SEGURIDAD INTERNA</t>
+        </is>
+      </c>
+      <c r="B251" s="0" t="inlineStr">
+        <is>
+          <t>EDUARDO LEYVA SIANKA</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO DE SEGURIDAD INTERNA</t>
+        </is>
+      </c>
+      <c r="B252" s="0" t="inlineStr">
         <is>
           <t>GERARDO  FERNÁNDEZ BORROTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="0" t="inlineStr">
+        <is>
+          <t>GRUPO DE SEGURIDAD INTERNA</t>
+        </is>
+      </c>
+      <c r="B253" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DAYLON  QUESADA  HECHAVARRÍA </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modificados:     formularios/form_calculo_utilidades.py Por terminar invalidantes(Disenno) 	modificados:     formularios/form_op_design.py     Terminado
</commit_message>
<xml_diff>
--- a/app-RRHH/file/evaluacion.xlsx
+++ b/app-RRHH/file/evaluacion.xlsx
@@ -1014,12 +1014,12 @@
     <row r="3" ht="15" customHeight="1" s="1">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GRUPO ALMACEN SIBONEY</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HERMINIO LAGARZA  ACOSTA</t>
+          <t>ARTURO EVASIO SÁNCHEZ  MARTÍNEZ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1041,12 +1041,12 @@
     <row r="4" ht="15" customHeight="1" s="1">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GRUPO TALLER BOYEROS</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DANIEL ALEJANDRO JIMENEZ BETANCOURT</t>
+          <t>MARITZA MOYA CUELLAR</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1068,22 +1068,22 @@
     <row r="5" ht="15" customHeight="1" s="1">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GRUPO TALLER BOYEROS</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>HENRY ROLANDO ESTEVEZ  CALDERÓN</t>
+          <t>ALEXANDER CARDOSA SALAZAR</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1095,12 +1095,12 @@
     <row r="6" ht="15" customHeight="1" s="1">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SUBDIRECCION TECNICA</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ISRAEL MORA  BELTRÁN</t>
+          <t>ONEDIS BASULTO HERNÁNDEZ</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1122,12 +1122,12 @@
     <row r="7" ht="15" customHeight="1" s="1">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SUBDIRECCION INFORMATICA</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DAUNIER HERNÁNDEZ  TRUJILLO</t>
+          <t>DILENIA HIDALGO SUÁREZ</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1149,17 +1149,17 @@
     <row r="8" ht="15" customHeight="1" s="1">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE DESARROLLO</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>YAILIN URRUTIA POMIER</t>
+          <t>ERIK LÁZARO PRENDES LAGO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1176,12 +1176,12 @@
     <row r="9" ht="15" customHeight="1" s="1">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SUBDIRECCION TECNICA</t>
+          <t>SUBDIRECCION COMERCIAL</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ALFREDO VAGNER PEÑA SILVA</t>
+          <t>JANETT ADRIANA VÁZQUEZ  FANEGO</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1203,44 +1203,44 @@
     <row r="10" ht="15" customHeight="1" s="1">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>SUBDIRECCION COMERCIAL</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ALEXANDER CARDOSA SALAZAR</t>
+          <t>ARIANNA PÉREZ  LLANO</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t xml:space="preserve">B </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>NE</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="1">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>SUBDIRECCION COMERCIAL</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ERIK LÁZARO PRENDES LAGO</t>
+          <t>JESSICA DE LAS MERCEDES DEL PESO ZAMBRANO</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1257,12 +1257,12 @@
     <row r="12" ht="15" customHeight="1" s="1">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>SUBDIRECCION COMERCIAL</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ARTURO EVASIO SÁNCHEZ  MARTÍNEZ</t>
+          <t>ADRIANA VALERA CORREA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1284,12 +1284,12 @@
     <row r="13" ht="15" customHeight="1" s="1">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>SUBDIRECCION COMERCIAL</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MARITZA MOYA CUELLAR</t>
+          <t>EDGAR SÁNCHEZ  OLIVA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1311,12 +1311,12 @@
     <row r="14" ht="15" customHeight="1" s="1">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>SUBDIRECCION COMERCIAL</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ONEDIS BASULTO HERNÁNDEZ</t>
+          <t>CLAUDIA LINARES  SOSA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1338,12 +1338,12 @@
     <row r="15" ht="15" customHeight="1" s="1">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>DILENIA HIDALGO SUÁREZ</t>
+          <t>JOSE FERMIN CORTIÑA PIÑERA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1365,66 +1365,66 @@
     <row r="16" ht="15" customHeight="1" s="1">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SUBDIRECCION COMERCIAL</t>
+          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ARIANNA PÉREZ  LLANO</t>
+          <t>LISANDRA HERNANDEZ CREACH</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="1">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SUBDIRECCION COMERCIAL</t>
+          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>JESSICA DE LAS MERCEDES DEL PESO ZAMBRANO</t>
+          <t>MAIYELIN  VERA VALDÉS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t xml:space="preserve">M </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>NE</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">B </t>
-        </is>
-      </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="1">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SUBDIRECCION COMERCIAL</t>
+          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ADRIANA VALERA CORREA</t>
+          <t>MARUCHA SERRET ROJAS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1434,24 +1434,24 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="1">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SUBDIRECCION COMERCIAL</t>
+          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>EDGAR SÁNCHEZ  OLIVA</t>
+          <t>ISIS IVETTE ESCALONA LEYVA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1473,12 +1473,12 @@
     <row r="20" ht="15" customHeight="1" s="1">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SUBDIRECCION COMERCIAL</t>
+          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CLAUDIA LINARES  SOSA</t>
+          <t>SUILEN REYES  SUÁREZ</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1505,12 +1505,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LISANDRA HERNANDEZ CREACH</t>
+          <t>DANIA BERETERVIDE  DOPICO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1527,17 +1527,17 @@
     <row r="22" ht="15" customHeight="1" s="1">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
+          <t>SUBDIRECCION DE ADMINISTRACION</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>JOSE FERMIN CORTIÑA PIÑERA</t>
+          <t>ABEL PRIETO CASQUERO</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1554,39 +1554,39 @@
     <row r="23" ht="15" customHeight="1" s="1">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
+          <t>SUBDIRECCION DE ADMINISTRACION</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MAIYELIN  VERA VALDÉS</t>
+          <t>JOSE LUIS CATURLA TERRY</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">M </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="1">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
+          <t>SUBDIRECCION DE ADMINISTRACION</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MARUCHA SERRET ROJAS</t>
+          <t>TERESA DE LA CARIDAD GARCÍA  BOLAÑOS</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1596,29 +1596,29 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="1">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
+          <t>SUBDIRECCION DE ADMINISTRACION</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ISIS IVETTE ESCALONA LEYVA</t>
+          <t>ADA DANIA GONZALEZ GONZALEZ</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1635,12 +1635,12 @@
     <row r="26" ht="15" customHeight="1" s="1">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
+          <t>SUBDIRECCION DE ADMINISTRACION</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SUILEN REYES  SUÁREZ</t>
+          <t>ERNESTO GUERRA MATA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1662,12 +1662,12 @@
     <row r="27" ht="15" customHeight="1" s="1">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SUBDIRECCION CONTABLE FINANCIERA</t>
+          <t>SUBDIRECCION DE ADMINISTRACION</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>DANIA BERETERVIDE  DOPICO</t>
+          <t>CARLOS  DIAZ ORDAZ</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>JOSE LUIS CATURLA TERRY</t>
+          <t>LEONARDO PEREZ RAMIREZ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1716,12 +1716,12 @@
     <row r="29" ht="15" customHeight="1" s="1">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
+          <t>SUBDIRECCION DE DESARROLLO</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>TERESA DE LA CARIDAD GARCÍA  BOLAÑOS</t>
+          <t>RAÚL PAVÓN  FUENTES</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1743,12 +1743,12 @@
     <row r="30" ht="15" customHeight="1" s="1">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
+          <t>SUBDIRECCION DE DESARROLLO</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ADA DANIA GONZALEZ GONZALEZ</t>
+          <t>YAILIN URRUTIA POMIER</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1770,17 +1770,17 @@
     <row r="31" ht="15" customHeight="1" s="1">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
+          <t>SUBDIRECCION DE DESARROLLO</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ABEL PRIETO CASQUERO</t>
+          <t>MARTHA BRENDA DÍAZ DELGADO</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1797,12 +1797,12 @@
     <row r="32" ht="15" customHeight="1" s="1">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
+          <t>SUBDIRECCION DE DESARROLLO</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ERNESTO GUERRA MATA</t>
+          <t>ALIUSKA LOURDES SANCHEZ HERNANDEZ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1824,12 +1824,12 @@
     <row r="33" ht="15" customHeight="1" s="1">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
+          <t>SUBDIRECCION DE DESARROLLO</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>CARLOS  DIAZ ORDAZ</t>
+          <t>DANAY GUZMÁN BORGES</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1851,12 +1851,12 @@
     <row r="34" ht="15" customHeight="1" s="1">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ADMINISTRACION</t>
+          <t>SUBDIRECCION INFORMATICA</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LEONARDO PEREZ RAMIREZ</t>
+          <t>FRANCISCO JAVIER CASTELLÓN  BARTROLI</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1878,12 +1878,12 @@
     <row r="35" ht="15" customHeight="1" s="1">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE DESARROLLO</t>
+          <t>SUBDIRECCION INFORMATICA</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MARTHA BRENDA DÍAZ DELGADO</t>
+          <t>EDUARDO  FORTE MARQUEZ</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1905,12 +1905,12 @@
     <row r="36" ht="15" customHeight="1" s="1">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE DESARROLLO</t>
+          <t>SUBDIRECCION INFORMATICA</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ALIUSKA LOURDES SANCHEZ HERNANDEZ</t>
+          <t>DAUNIER HERNÁNDEZ  TRUJILLO</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1932,12 +1932,12 @@
     <row r="37" ht="15" customHeight="1" s="1">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE DESARROLLO</t>
+          <t>SUBDIRECCION INFORMATICA</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>DANAY GUZMÁN BORGES</t>
+          <t>RANNIEL RIVERO SEVILA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1959,12 +1959,12 @@
     <row r="38" ht="15" customHeight="1" s="1">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE DESARROLLO</t>
+          <t>SUBDIRECCION INFORMATICA</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>RAÚL PAVÓN  FUENTES</t>
+          <t>ALEJANDRO  RAMÍREZ COMESAÑAS</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1986,12 +1986,12 @@
     <row r="39" ht="15" customHeight="1" s="1">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SUBDIRECCION INFORMATICA</t>
+          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ALEJANDRO  RAMÍREZ COMESAÑAS</t>
+          <t>YAMILA JO  MARRERO</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2013,12 +2013,12 @@
     <row r="40" ht="15" customHeight="1" s="1">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SUBDIRECCION INFORMATICA</t>
+          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>FRANCISCO JAVIER CASTELLÓN  BARTROLI</t>
+          <t>HASLEMER SOTOLONGO  CUZA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2040,12 +2040,12 @@
     <row r="41" ht="15" customHeight="1" s="1">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SUBDIRECCION INFORMATICA</t>
+          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>EDUARDO  FORTE MARQUEZ</t>
+          <t>REMBERTO GONZÁLEZ MORALES</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2067,12 +2067,12 @@
     <row r="42" ht="15" customHeight="1" s="1">
       <c r="A42" t="inlineStr">
         <is>
-          <t>SUBDIRECCION INFORMATICA</t>
+          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>RANNIEL RIVERO SEVILA</t>
+          <t>ROGER ONDARSE ROJAS</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2082,12 +2082,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>HASLEMER SOTOLONGO  CUZA</t>
+          <t>ROBERTO PADILLA  COLAO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2121,12 +2121,12 @@
     <row r="44" ht="15" customHeight="1" s="1">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
+          <t>GRUPO ALMACEN SIBONEY</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>REMBERTO GONZÁLEZ MORALES</t>
+          <t>ROLANDO RODRIGUEZ GONZALEZ</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2148,12 +2148,12 @@
     <row r="45" ht="15" customHeight="1" s="1">
       <c r="A45" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
+          <t>GRUPO ALMACEN SIBONEY</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ROGER ONDARSE ROJAS</t>
+          <t>ERNESTO SÁNCHEZ  COLUMBIÉ</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2163,24 +2163,24 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="1">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
+          <t>GRUPO ALMACEN SIBONEY</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ROBERTO PADILLA  COLAO</t>
+          <t>ALEJANDRO MONTAÑA  RIVERA</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2190,7 +2190,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2202,12 +2202,12 @@
     <row r="47" ht="15" customHeight="1" s="1">
       <c r="A47" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE ASEGURAMIENTO</t>
+          <t>GRUPO ALMACEN SIBONEY</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>YAMILA JO  MARRERO</t>
+          <t>HERMINIO LAGARZA  ACOSTA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2229,12 +2229,12 @@
     <row r="48" ht="15" customHeight="1" s="1">
       <c r="A48" t="inlineStr">
         <is>
-          <t>GRUPO ALMACEN SIBONEY</t>
+          <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ALEJANDRO MONTAÑA  RIVERA</t>
+          <t>LÁZARO REINIER RODRÍGUEZ RAVELO</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2256,12 +2256,12 @@
     <row r="49" ht="15" customHeight="1" s="1">
       <c r="A49" t="inlineStr">
         <is>
-          <t>GRUPO ALMACEN SIBONEY</t>
+          <t>SUBDIRECCION DE OPERACIONES</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ERNESTO SÁNCHEZ  COLUMBIÉ</t>
+          <t>ALEXEI BERNIS VILTRES</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2271,12 +2271,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
@@ -2639,12 +2639,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>LÁZARO REINIER RODRÍGUEZ RAVELO</t>
+          <t>LUIS ALBERTO PITA BODAÑO</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2666,12 +2666,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>LUIS ALBERTO PITA BODAÑO</t>
+          <t>OSMAR MANUEL VAILLANT QUEZADA</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2693,7 +2693,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>OSMAR MANUEL VAILLANT QUEZADA</t>
+          <t>YANSEL GONZALEZ VARELA</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2720,7 +2720,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>YANSEL GONZALEZ VARELA</t>
+          <t>DANIEL SANTIAGO RAMOS VALLS</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2730,7 +2730,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2747,7 +2747,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DANIEL SANTIAGO RAMOS VALLS</t>
+          <t>BENIGNO GONZALEZ ORTIZ</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2774,7 +2774,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>BENIGNO GONZALEZ ORTIZ</t>
+          <t>ARIEL PEÑA  NAPOLES</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ARIEL PEÑA  NAPOLES</t>
+          <t>DIMAS MARCOS IBALBIA PAIROL</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DIMAS MARCOS IBALBIA PAIROL</t>
+          <t>EMIGDIO JIMÉNEZ PEÑA</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>EMIGDIO JIMÉNEZ PEÑA</t>
+          <t>JUAN ALEXANDER  ALBUQUERQUE HERRERA</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>JUAN ALEXANDER  ALBUQUERQUE HERRERA</t>
+          <t>NOEL FERNÁNDEZ VARELA</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2909,12 +2909,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>NOEL FERNÁNDEZ VARELA</t>
+          <t>OSMEL LEONARDO ZAMORA PEREZ</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2924,24 +2924,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" s="1">
       <c r="A74" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE OPERACIONES</t>
+          <t>SUBDIRECCION TECNICA</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>OSMEL LEONARDO ZAMORA PEREZ</t>
+          <t>ALFREDO VAGNER PEÑA SILVA</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2951,7 +2951,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>RAMÓN OQUENDO  FADRAGA</t>
+          <t>JUAN CARLOS YAMACHO SILVA</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>JUAN CARLOS YAMACHO SILVA</t>
+          <t>YEAN MARC MORENO  CABRERA</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3005,7 +3005,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>MB</t>
         </is>
       </c>
     </row>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>YEAN MARC MORENO  CABRERA</t>
+          <t>RAMÓN OQUENDO  FADRAGA</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3032,29 +3032,29 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>MB</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="78" ht="15" customHeight="1" s="1">
       <c r="A78" t="inlineStr">
         <is>
-          <t>GRUPO TALLER BOYEROS</t>
+          <t>SUBDIRECCION TECNICA</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>MAIQUEL CONCEPCION PADILLA</t>
+          <t>ISRAEL MORA  BELTRÁN</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3071,22 +3071,22 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>REINIER ESTRADA VIVES</t>
+          <t>IVAN  CRUZ GARCIA</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
@@ -3098,7 +3098,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ALDO  OLIVEROS  CRUZ</t>
+          <t>EDDY RODRIGUEZ RODRIGUEZ</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>IVAN  CRUZ GARCIA</t>
+          <t>ANGEL DANIEL PASCUAL  VALDÉS</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>EDDY RODRIGUEZ RODRIGUEZ</t>
+          <t>ALEJANDRO BATISTA  CRUZ</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>EDDY RODRÍGUEZ CARBALLEDO</t>
+          <t>DANIEL ALEJANDRO JIMENEZ BETANCOURT</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>ALEJANDRO BATISTA  CRUZ</t>
+          <t>EDDY RODRÍGUEZ CARBALLEDO</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3228,12 +3228,12 @@
     <row r="85" ht="15" customHeight="1" s="1">
       <c r="A85" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
+          <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>VALIA NOGUERA FIGUEROA</t>
+          <t>HENRY ROLANDO ESTEVEZ  CALDERÓN</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3255,22 +3255,22 @@
     <row r="86" ht="15" customHeight="1" s="1">
       <c r="A86" t="inlineStr">
         <is>
-          <t>GRUPO TALLER SIBONEY</t>
+          <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>YURY ROBERTO CONYEDO ALEJO</t>
+          <t>MAIQUEL CONCEPCION PADILLA</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -3282,39 +3282,39 @@
     <row r="87" ht="15" customHeight="1" s="1">
       <c r="A87" t="inlineStr">
         <is>
-          <t>GRUPO TALLER SIBONEY</t>
+          <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>LUIS BULNES  CARRILLO</t>
+          <t>REINIER ESTRADA VIVES</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1" s="1">
       <c r="A88" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
+          <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>ANA JULIA GONZÁLEZ GÓMEZ</t>
+          <t>ALDO  OLIVEROS  CRUZ</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3336,39 +3336,39 @@
     <row r="89" ht="15" customHeight="1" s="1">
       <c r="A89" t="inlineStr">
         <is>
-          <t>GRUPO TALLER SIBONEY</t>
+          <t>GRUPO TALLER BOYEROS</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>REINALDO RAMOS  GÓMEZ</t>
+          <t>JOAQUIN MODESTO PERDOMO PEREZ</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
     <row r="90" ht="15" customHeight="1" s="1">
       <c r="A90" t="inlineStr">
         <is>
-          <t>GRUPO TALLER SIBONEY</t>
+          <t>GRUPO TALLER HABANA</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>YANET DEVESA  SÁNCHEZ</t>
+          <t>JUAN DE LEÓN  CARMENATY</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3390,12 +3390,12 @@
     <row r="91" ht="15" customHeight="1" s="1">
       <c r="A91" t="inlineStr">
         <is>
-          <t>GRUPO TALLER SIBONEY</t>
+          <t>GRUPO TALLER HABANA</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>LUIS DANIEL GONZÁLEZ  VIERA</t>
+          <t>IBRAHIN FERRER  DE LA ROSA</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3417,12 +3417,12 @@
     <row r="92" ht="15" customHeight="1" s="1">
       <c r="A92" t="inlineStr">
         <is>
-          <t>GRUPO TALLER SIBONEY</t>
+          <t>GRUPO TALLER HABANA</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>JUAN CARLOS TRELLES  CABRERA</t>
+          <t>WILLIAN RODRÍGUEZ VELIZ</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3444,12 +3444,12 @@
     <row r="93" ht="15" customHeight="1" s="1">
       <c r="A93" t="inlineStr">
         <is>
-          <t>GRUPO TALLER SIBONEY</t>
+          <t>GRUPO TALLER HABANA</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>MALKIEL  MOJENA HERNANDEZ</t>
+          <t>MIGUEL VALLE  ÁLVAREZ</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>YASSER BOTELLO VIDAL</t>
+          <t>LAZARO YORDAN VALDES BRUNET</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3491,7 +3491,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
     </row>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>YASER RENE LOPEZ BLANCO</t>
+          <t>CARLOS WILFREDO AROZARENA CORTES</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
     </row>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>ANTUAN UMPIERRE ALVAREZ</t>
+          <t>ARMANDO LOPEZ GUERRA</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3557,7 +3557,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>RICARDO DANIEL PÉREZ  ALLISON</t>
+          <t>JEIBEL ALONSO SARDIÑAS</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
     </row>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>LEONARDO RODRÍGUEZ  MEDINA</t>
+          <t>KEVIN SORRELL GARCIA</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3599,56 +3599,56 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>MB</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="99" ht="15" customHeight="1" s="1">
       <c r="A99" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
+          <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>ESTEBAN DAVID SÁNCHEZ  NOVO</t>
+          <t>EDUARDO CALDERON FUENTES</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
     </row>
     <row r="100" ht="15" customHeight="1" s="1">
       <c r="A100" t="inlineStr">
         <is>
-          <t>GRUPO TALLER HABANA</t>
+          <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>MIGUEL VALLE  ÁLVAREZ</t>
+          <t>JUAN ANTONIO HERNANDEZ RAMIREZ</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3660,12 +3660,12 @@
     <row r="101" ht="15" customHeight="1" s="1">
       <c r="A101" t="inlineStr">
         <is>
-          <t>GRUPO TALLER HABANA</t>
+          <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>JUAN DE LEÓN  CARMENATY</t>
+          <t>DANIEL MUÑOZ GONZÁLEZ</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3680,19 +3680,19 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>MB</t>
         </is>
       </c>
     </row>
     <row r="102" ht="15" customHeight="1" s="1">
       <c r="A102" t="inlineStr">
         <is>
-          <t>GRUPO TALLER HABANA</t>
+          <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>IBRAHIN FERRER  DE LA ROSA</t>
+          <t>ROBERTO FRANCISCO JARDÓN  PRENDES</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3714,12 +3714,12 @@
     <row r="103" ht="15" customHeight="1" s="1">
       <c r="A103" t="inlineStr">
         <is>
-          <t>GRUPO TALLER HABANA</t>
+          <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>WILLIAN RODRÍGUEZ VELIZ</t>
+          <t>YOESLAN  VALDES SANCHEZ</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>JULIO ALFREDO WONG SERRA</t>
+          <t>YURY ROBERTO CONYEDO ALEJO</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>JORGE LUIS LÓPEZ  ORTA</t>
+          <t>LUIS BULNES  CARRILLO</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
     </row>
@@ -3800,12 +3800,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>ERNESTO ALARCÓN  ESPINOSA</t>
+          <t>REINALDO RAMOS  GÓMEZ</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>HUMBERTO PABLO CABEZAS   ALONSO</t>
+          <t>YANET DEVESA  SÁNCHEZ</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3854,7 +3854,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>YORGENIS RAMÍREZ  VELÁZQUEZ</t>
+          <t>LUIS DANIEL GONZÁLEZ  VIERA</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>RAIDEL RAMOS ARREBATO</t>
+          <t>JUAN CARLOS TRELLES  CABRERA</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3896,7 +3896,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>ERANDIS  ALVAREZ GARCIA</t>
+          <t>MALKIEL  MOJENA HERNANDEZ</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3935,7 +3935,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>LAZARO YORDAN VALDES BRUNET</t>
+          <t>YASSER BOTELLO VIDAL</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
@@ -3962,7 +3962,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>CARLOS WILFREDO AROZARENA CORTES</t>
+          <t>YASER RENE LOPEZ BLANCO</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3977,7 +3977,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>ARMANDO LOPEZ GUERRA</t>
+          <t>ANTUAN UMPIERRE ALVAREZ</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4016,7 +4016,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>JEIBEL ALONSO SARDIÑAS</t>
+          <t>RICARDO DANIEL PÉREZ  ALLISON</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4031,7 +4031,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
@@ -4043,7 +4043,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>KEVIN SORRELL GARCIA</t>
+          <t>LEONARDO RODRÍGUEZ  MEDINA</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>MB</t>
         </is>
       </c>
     </row>
@@ -4070,22 +4070,22 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>EDUARDO CALDERON FUENTES</t>
+          <t>JULIO ALFREDO WONG SERRA</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
@@ -4097,17 +4097,17 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>JUAN ANTONIO HERNANDEZ RAMIREZ</t>
+          <t>JORGE LUIS LÓPEZ  ORTA</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>DANIEL MUÑOZ GONZÁLEZ</t>
+          <t>ERNESTO ALARCÓN  ESPINOSA</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>MB</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>ROBERTO FRANCISCO JARDÓN  PRENDES</t>
+          <t>HUMBERTO PABLO CABEZAS   ALONSO</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4173,12 +4173,12 @@
     <row r="120" ht="15" customHeight="1" s="1">
       <c r="A120" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
+          <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>PABLO PÉREZ  TORRES</t>
+          <t>YORGENIS RAMÍREZ  VELÁZQUEZ</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4200,12 +4200,12 @@
     <row r="121" ht="15" customHeight="1" s="1">
       <c r="A121" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
+          <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>IDARMIS RIVERA  LEÓN</t>
+          <t>RAIDEL RAMOS ARREBATO</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4220,19 +4220,19 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
     </row>
     <row r="122" ht="15" customHeight="1" s="1">
       <c r="A122" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
+          <t>GRUPO TALLER SIBONEY</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>ARMINDA JULIA ARIAS  HERNÁNDEZ</t>
+          <t>ERANDIS  ALVAREZ GARCIA</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4259,7 +4259,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>RODOBALDO DÍAZ  ARTEAGA</t>
+          <t>YANOSKY ESCAÑO  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>ORLANDO LLANES  MESA</t>
+          <t>VALIA NOGUERA FIGUEROA</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>JESUS BARCELONA  ALAMBARES</t>
+          <t>ANA JULIA GONZÁLEZ GÓMEZ</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>EDUARDO GONZÁLEZ  FERNÁNDEZ</t>
+          <t>ESTEBAN DAVID SÁNCHEZ  NOVO</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4367,7 +4367,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>YUNIERT CUTIÑO  GRIÑAN</t>
+          <t>PABLO PÉREZ  TORRES</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>LEONEL SILVA  ABAD</t>
+          <t>IDARMIS RIVERA  LEÓN</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>CONSUELO GONZÁLEZ  DÍAZ</t>
+          <t>ARMINDA JULIA ARIAS  HERNÁNDEZ</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>OSMEL DÍAZ  CRUZ</t>
+          <t>RODOBALDO DÍAZ  ARTEAGA</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4475,7 +4475,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>JULIO CÉSAR ESCAÑO  RODRÍGUEZ</t>
+          <t>ORLANDO LLANES  MESA</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4502,7 +4502,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>ALAIN MERCHÁN  OLIVA</t>
+          <t>JESUS BARCELONA  ALAMBARES</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4529,7 +4529,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>JORGE ALBERTO GOENAGA  MARTÍNEZ</t>
+          <t>EDUARDO GONZÁLEZ  FERNÁNDEZ</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>DENNIS ORTIZ  HERNÁNDEZ</t>
+          <t>YUNIERT CUTIÑO  GRIÑAN</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4583,7 +4583,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>JULIO CESAR BERMUDEZ  LOPEZ</t>
+          <t>LEONEL SILVA  ABAD</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>YANOSKY ESCAÑO  RODRÍGUEZ</t>
+          <t>CONSUELO GONZÁLEZ  DÍAZ</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>RAYWER SIERRA  RODRÍGUEZ</t>
+          <t>OSMEL DÍAZ  CRUZ</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4664,7 +4664,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>JONAH LÓPEZ  DÍAZ</t>
+          <t>JULIO CÉSAR ESCAÑO  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4691,7 +4691,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>YADIRA FERRARI  SUÁREZ</t>
+          <t>ALAIN MERCHÁN  OLIVA</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>MAIKEL CÓRDOVA  GÓNGORA</t>
+          <t>JORGE ALBERTO GOENAGA  MARTÍNEZ</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>OSMEL IGNACIO FERNÁNDEZ  CAMPILLO</t>
+          <t>DENNIS ORTIZ  HERNÁNDEZ</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>LIVIO AVELINO LIMONTA JIMENEZ</t>
+          <t>JULIO CESAR BERMUDEZ  LOPEZ</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4799,12 +4799,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>YAN LUIS MARTINEZ GONZALEZ</t>
+          <t>RAYWER SIERRA  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4826,12 +4826,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>YAZMANY ANTONIO COTILLA HERNANDEZ</t>
+          <t>JONAH LÓPEZ  DÍAZ</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>MAXIMO MENDEZ MOLINA</t>
+          <t>YADIRA FERRARI  SUÁREZ</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4880,7 +4880,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>ANAEVI MARTÍNEZ  RAMOS</t>
+          <t>MAIKEL CÓRDOVA  GÓNGORA</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4907,7 +4907,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>KENIA AMINTA DELGADO  RODRÍGUEZ</t>
+          <t>OSMEL IGNACIO FERNÁNDEZ  CAMPILLO</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4934,7 +4934,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>ALAIN GARCÍA  JEREZ</t>
+          <t>LIVIO AVELINO LIMONTA JIMENEZ</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4961,12 +4961,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>ARIANNA GUZMÁN RIVERO</t>
+          <t>YAN LUIS MARTINEZ GONZALEZ</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4988,12 +4988,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>SANDOR RUBÉN  ROLDÁN</t>
+          <t>YAZMANY ANTONIO COTILLA HERNANDEZ</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -5015,7 +5015,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>YAMILKA DE LA CARIDAD SOSA  REMÓN</t>
+          <t>MAXIMO MENDEZ MOLINA</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>LUIS ANGEL GARCÍA ALARCÓN</t>
+          <t>ANAEVI MARTÍNEZ  RAMOS</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -5069,7 +5069,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>VIRGINIA ISABEL SOTO  CASTRO</t>
+          <t>KENIA AMINTA DELGADO  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -5096,7 +5096,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>MIGUEL ANGEL CÁRDENAS  FERNÁNDEZ</t>
+          <t>ALAIN GARCÍA  JEREZ</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -5123,7 +5123,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>ELIEZER SENÉN MEDINA  CARBONELL</t>
+          <t>ARIANNA GUZMÁN RIVERO</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>YOEL MONDUY  RODRÍGUEZ</t>
+          <t>SANDOR RUBÉN  ROLDÁN</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>YUSNIEL MOJENA  CAMPILLO</t>
+          <t>YAMILKA DE LA CARIDAD SOSA  REMÓN</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -5204,7 +5204,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>DANCÉS LEÓN  HERRERA</t>
+          <t>LUIS ANGEL GARCÍA ALARCÓN</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -5231,7 +5231,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>JULIO ESTEBAN FIGUEREDO  DEL TORO</t>
+          <t>VIRGINIA ISABEL SOTO  CASTRO</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -5253,12 +5253,12 @@
     <row r="160" ht="15" customHeight="1" s="1">
       <c r="A160" t="inlineStr">
         <is>
-          <t>GRUPO DE VENTAS PINAR DEL RIO</t>
+          <t>DEPARTAMENTO AEROPUERTO</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>FRANCISCO PALACIOS CABRERA</t>
+          <t>MIGUEL ANGEL CÁRDENAS  FERNÁNDEZ</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -5280,12 +5280,12 @@
     <row r="161" ht="15" customHeight="1" s="1">
       <c r="A161" t="inlineStr">
         <is>
-          <t>GRUPO DE VENTAS PINAR DEL RIO</t>
+          <t>DEPARTAMENTO AEROPUERTO</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>LUIS MANUEL PUENTES  CID</t>
+          <t>ELIEZER SENÉN MEDINA  CARBONELL</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -5307,12 +5307,12 @@
     <row r="162" ht="15" customHeight="1" s="1">
       <c r="A162" t="inlineStr">
         <is>
-          <t>GRUPO DE VENTAS PINAR DEL RIO</t>
+          <t>DEPARTAMENTO AEROPUERTO</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>PEDRO BEC LÓPEZ</t>
+          <t>YOEL MONDUY  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -5334,12 +5334,12 @@
     <row r="163" ht="15" customHeight="1" s="1">
       <c r="A163" t="inlineStr">
         <is>
-          <t>GRUPO DE VENTAS PINAR DEL RIO</t>
+          <t>DEPARTAMENTO AEROPUERTO</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>ADOLFO DAMIÁN MORENO GONZÁLEZ</t>
+          <t>YUSNIEL MOJENA  CAMPILLO</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -5349,7 +5349,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -5361,12 +5361,12 @@
     <row r="164" ht="15" customHeight="1" s="1">
       <c r="A164" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIUDAD</t>
+          <t>DEPARTAMENTO AEROPUERTO</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>MANUEL RAÚL GÓMEZ  FERRO</t>
+          <t>DANCÉS LEÓN  HERRERA</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -5388,12 +5388,12 @@
     <row r="165" ht="15" customHeight="1" s="1">
       <c r="A165" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIUDAD</t>
+          <t>DEPARTAMENTO AEROPUERTO</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>AVELARDO IZQUIERDO  REYES</t>
+          <t>JULIO ESTEBAN FIGUEREDO  DEL TORO</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -5415,12 +5415,12 @@
     <row r="166" ht="15" customHeight="1" s="1">
       <c r="A166" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIUDAD</t>
+          <t>DEPARTAMENTO AEROPUERTO</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>YOASMIN CALDERON  PÉREZ</t>
+          <t>BÁRBARO PABLO GONZÁLEZ  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -5442,17 +5442,17 @@
     <row r="167" ht="15" customHeight="1" s="1">
       <c r="A167" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIENFUEGOS</t>
+          <t>DEPARTAMENTO AEROPUERTO</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>MAIKEL YUDIANNY  JIMÉNEZ  PÉREZ</t>
+          <t>MARIA DEL  CARMEN CASTAÑER  AVERHOFF</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -5469,12 +5469,12 @@
     <row r="168" ht="15" customHeight="1" s="1">
       <c r="A168" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>GRUPO DE VENTAS PINAR DEL RIO</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>ANNIER  CHAVEZ  LECTO</t>
+          <t>PEDRO BEC LÓPEZ</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -5496,12 +5496,12 @@
     <row r="169" ht="15" customHeight="1" s="1">
       <c r="A169" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+          <t>GRUPO DE VENTAS PINAR DEL RIO</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>MARTINIANO HERNÁNDEZ  BARCELÓ</t>
+          <t>ADOLFO DAMIÁN MORENO GONZÁLEZ</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -5523,12 +5523,12 @@
     <row r="170" ht="15" customHeight="1" s="1">
       <c r="A170" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>GRUPO DE VENTAS PINAR DEL RIO</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>ALFREDO IGARZA  BARRIEL</t>
+          <t>FRANCISCO PALACIOS CABRERA</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -5550,12 +5550,12 @@
     <row r="171" ht="15" customHeight="1" s="1">
       <c r="A171" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO VILLA CLARA</t>
+          <t>GRUPO DE VENTAS PINAR DEL RIO</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>ANA MARIA HERNÁNDEZ  GONZÁLEZ</t>
+          <t>LUIS MANUEL PUENTES  CID</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5577,12 +5577,12 @@
     <row r="172" ht="15" customHeight="1" s="1">
       <c r="A172" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+          <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>INELDO IDEL ESPINOSA GARCIA</t>
+          <t>AVELARDO IZQUIERDO  REYES</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5604,12 +5604,12 @@
     <row r="173" ht="15" customHeight="1" s="1">
       <c r="A173" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>YOSVANY PRIETO  MERIÑO</t>
+          <t>YUDITH REMIS  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -5636,7 +5636,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>PEDRO EMILIO CARNOT  PEREIRA</t>
+          <t>ALEXIS SUÁREZ  CAPOTE</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>YUDITH REMIS  RODRÍGUEZ</t>
+          <t>ENID CRESPO  TORRES</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -5690,7 +5690,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>ALEXIS SUÁREZ  CAPOTE</t>
+          <t>OSVALDO MORENO  HERNÁNDEZ</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -5717,7 +5717,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>ENID CRESPO  TORRES</t>
+          <t>DARIEL ORTIZ VALDEZ</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -5744,7 +5744,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>OSVALDO MORENO  HERNÁNDEZ</t>
+          <t>JULIO GERMÁN MORA NEGRÍN</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -5754,7 +5754,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -5771,7 +5771,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>DARIEL ORTIZ VALDEZ</t>
+          <t>PEDRO EMILIO CARNOT  PEREIRA</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -5798,7 +5798,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>JULIO GERMÁN MORA NEGRÍN</t>
+          <t>YOASMIN CALDERON  PÉREZ</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -5808,7 +5808,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -5874,12 +5874,12 @@
     <row r="183" ht="15" customHeight="1" s="1">
       <c r="A183" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO VARADERO</t>
+          <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>YUDIETH PALENZUELA  YANES</t>
+          <t>MANUEL RAÚL GÓMEZ  FERRO</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5901,12 +5901,12 @@
     <row r="184" ht="15" customHeight="1" s="1">
       <c r="A184" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO VARADERO</t>
+          <t>DEPARTAMENTO CIUDAD</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>SHEYLA NORES  GONZÁLEZ</t>
+          <t>LOYSLI REINALDO CORDERO GÓMEZ</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>JAVIEL PITA  CABALLERO</t>
+          <t>JOAQUÍN FERNÁNDEZ  RONDÓN</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -5960,7 +5960,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>MICHAEL DE ARMAS  RODRÍGUEZ</t>
+          <t>YUDIETH PALENZUELA  YANES</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -5987,7 +5987,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>ARTURO DÁVALOS  MOROS</t>
+          <t>SHEYLA NORES  GONZÁLEZ</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -6014,7 +6014,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>JOAQUÍN FERNÁNDEZ  RONDÓN</t>
+          <t>JAVIEL PITA  CABALLERO</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -6041,7 +6041,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>LUIS ANTONIO NARANJO  QUINTANA</t>
+          <t>MICHAEL DE ARMAS  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>YOAN  HERNÁNDEZ  MENDEZ</t>
+          <t>ARTURO DÁVALOS  MOROS</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -6095,12 +6095,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>LIUSKA ORTEGA  RODRIGUEZ</t>
+          <t>LUIS ANTONIO NARANJO  QUINTANA</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -6122,7 +6122,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>JOSE MIGUEL NAVARRO CRUZ</t>
+          <t>YOAN  HERNÁNDEZ  MENDEZ</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -6149,12 +6149,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>DIOSDADO VIZCAINO  RODRÍGUEZ</t>
+          <t>LIUSKA ORTEGA  RODRIGUEZ</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -6176,7 +6176,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>MARIANELA MANCHA TARAJANO</t>
+          <t>JOSE MIGUEL NAVARRO CRUZ</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>MAILYN LORENZO  RODRÍGUEZ</t>
+          <t>DIOSDADO VIZCAINO  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -6213,24 +6213,24 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="196" ht="15" customHeight="1" s="1">
       <c r="A196" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO VILLA CLARA</t>
+          <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>FÉLIX MEDINA  SUÁREZ</t>
+          <t>MARIANELA MANCHA TARAJANO</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -6252,12 +6252,12 @@
     <row r="197" ht="15" customHeight="1" s="1">
       <c r="A197" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO VILLA CLARA</t>
+          <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>EVIS ACUÑA BRAVO</t>
+          <t>MAILYN LORENZO  RODRÍGUEZ</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -6267,34 +6267,34 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
     <row r="198" ht="15" customHeight="1" s="1">
       <c r="A198" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO VILLA CLARA</t>
+          <t>DEPARTAMENTO VARADERO</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>EDEL JIMÉNEZ  ALBA</t>
+          <t>JOSE FRANCISCO DUQUESNE BAEZ</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -6549,12 +6549,12 @@
     <row r="208" ht="15" customHeight="1" s="1">
       <c r="A208" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIENFUEGOS</t>
+          <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>ALFONSO COLINA  HURTADO</t>
+          <t>ANA MARIA HERNÁNDEZ  GONZÁLEZ</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -6576,12 +6576,12 @@
     <row r="209" ht="15" customHeight="1" s="1">
       <c r="A209" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIENFUEGOS</t>
+          <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>JESUS RAFAEL  DELGADO GESSA</t>
+          <t>EVIS ACUÑA BRAVO</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -6603,12 +6603,12 @@
     <row r="210" ht="15" customHeight="1" s="1">
       <c r="A210" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIENFUEGOS</t>
+          <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>ROLANDO GÓMEZ  SERRANO</t>
+          <t>FÉLIX MEDINA  SUÁREZ</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -6630,12 +6630,12 @@
     <row r="211" ht="15" customHeight="1" s="1">
       <c r="A211" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIENFUEGOS</t>
+          <t>DEPARTAMENTO VILLA CLARA</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>ADEL  FERNANDEZ GONZALEZ</t>
+          <t>EDEL JIMÉNEZ  ALBA</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -6711,12 +6711,12 @@
     <row r="214" ht="15" customHeight="1" s="1">
       <c r="A214" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+          <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>GEORLANDY  VENEGA SANTOS</t>
+          <t>LUIS ANGEL YERA PEREZ</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -6738,17 +6738,17 @@
     <row r="215" ht="15" customHeight="1" s="1">
       <c r="A215" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+          <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>ABUNDIO MOYA  PÉREZ</t>
+          <t>MAIKEL YUDIANNY  JIMÉNEZ  PÉREZ</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -6765,12 +6765,12 @@
     <row r="216" ht="15" customHeight="1" s="1">
       <c r="A216" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+          <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t xml:space="preserve">JOSE CARLOS  SANCHEZ  CID </t>
+          <t>ALFONSO COLINA  HURTADO</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -6792,12 +6792,12 @@
     <row r="217" ht="15" customHeight="1" s="1">
       <c r="A217" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+          <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>JUAN CARLOS ABDALA  GARCÍA</t>
+          <t>JESUS RAFAEL  DELGADO GESSA</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -6819,17 +6819,17 @@
     <row r="218" ht="15" customHeight="1" s="1">
       <c r="A218" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+          <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>ALYS GARCÍA  HERNÁNDEZ</t>
+          <t>ROLANDO GÓMEZ  SERRANO</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
@@ -6839,19 +6839,19 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="219" ht="15" customHeight="1" s="1">
       <c r="A219" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CAMAGUEY</t>
+          <t>DEPARTAMENTO CIENFUEGOS</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>ALEXIS ELIA CASTILLO  JIMÉNEZ</t>
+          <t>ADEL  FERNANDEZ GONZALEZ</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -6873,17 +6873,17 @@
     <row r="220" ht="15" customHeight="1" s="1">
       <c r="A220" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CAMAGUEY</t>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>DUANY RICHARD VIGO MARRERO</t>
+          <t>ALYS GARCÍA  HERNÁNDEZ</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
@@ -6893,19 +6893,19 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
     <row r="221" ht="15" customHeight="1" s="1">
       <c r="A221" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CAMAGUEY</t>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>HECTOR EUTIQUIO MOYARES  RAMOS</t>
+          <t>MARTINIANO HERNÁNDEZ  BARCELÓ</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -6927,12 +6927,12 @@
     <row r="222" ht="15" customHeight="1" s="1">
       <c r="A222" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CAMAGUEY</t>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>ADRIÁN RODRÍGUEZ BARRERAS</t>
+          <t>INELDO IDEL ESPINOSA GARCIA</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -6954,12 +6954,12 @@
     <row r="223" ht="15" customHeight="1" s="1">
       <c r="A223" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CAMAGUEY</t>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>ERIBERTO RAÚL VALDÉS  FONTELA</t>
+          <t>GEORLANDY  VENEGA SANTOS</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -6981,12 +6981,12 @@
     <row r="224" ht="15" customHeight="1" s="1">
       <c r="A224" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CAMAGUEY</t>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>PATRICIO HERNÁNDEZ  FÁBREGAS</t>
+          <t>ABUNDIO MOYA  PÉREZ</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -7008,12 +7008,12 @@
     <row r="225" ht="15" customHeight="1" s="1">
       <c r="A225" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>RACIEL PEREDA AGUILERA</t>
+          <t xml:space="preserve">JOSE CARLOS  SANCHEZ  CID </t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -7035,22 +7035,22 @@
     <row r="226" ht="15" customHeight="1" s="1">
       <c r="A226" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>PEDRO RAFAEL ALDANA ZAPATA</t>
+          <t>JUAN CARLOS ABDALA  GARCÍA</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
@@ -7062,39 +7062,39 @@
     <row r="227" ht="15" customHeight="1" s="1">
       <c r="A227" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CIEGO DE AVILA</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>CARLOS COBIRLLA AGUILERA</t>
+          <t>EMILIO  VIÑALES  FIGUEROA</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="228" ht="15" customHeight="1" s="1">
       <c r="A228" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>OSMANIS FERNANDEZ ANZARDO</t>
+          <t>ALEXIS ELIA CASTILLO  JIMÉNEZ</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -7116,12 +7116,12 @@
     <row r="229" ht="15" customHeight="1" s="1">
       <c r="A229" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>ALEXIS RODRÍGUEZ CARRALERO</t>
+          <t>DUANY RICHARD VIGO MARRERO</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -7143,12 +7143,12 @@
     <row r="230" ht="15" customHeight="1" s="1">
       <c r="A230" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>JORGE LUIS SAAVEDRA  GARCÍA</t>
+          <t>HECTOR EUTIQUIO MOYARES  RAMOS</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -7170,12 +7170,12 @@
     <row r="231" ht="15" customHeight="1" s="1">
       <c r="A231" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>NESTOR ERITH HERNÁNDEZ  MENA</t>
+          <t>ADRIÁN RODRÍGUEZ BARRERAS</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -7185,24 +7185,24 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="232" ht="15" customHeight="1" s="1">
       <c r="A232" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>LUIS ROBERTO ALMAGUER  SOLIS</t>
+          <t>ERIBERTO RAÚL VALDÉS  FONTELA</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -7224,12 +7224,12 @@
     <row r="233" ht="15" customHeight="1" s="1">
       <c r="A233" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO HOLGUIN</t>
+          <t>DEPARTAMENTO CAMAGUEY</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>LIDISMIR DOROTEA VEGA  ARENA</t>
+          <t>PATRICIO HERNÁNDEZ  FÁBREGAS</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -7359,12 +7359,12 @@
     <row r="238" ht="15" customHeight="1" s="1">
       <c r="A238" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>ARNULFO EDGAR LUNA  MENDOZA</t>
+          <t>OSMANIS FERNANDEZ ANZARDO</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -7386,12 +7386,12 @@
     <row r="239" ht="15" customHeight="1" s="1">
       <c r="A239" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>JOSE ALAIN MASSO  ALMENARES</t>
+          <t>ALEXIS RODRÍGUEZ CARRALERO</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -7413,12 +7413,12 @@
     <row r="240" ht="15" customHeight="1" s="1">
       <c r="A240" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>DIUNEIKY GIRÓN  NOA</t>
+          <t>JORGE LUIS SAAVEDRA  GARCÍA</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -7440,12 +7440,12 @@
     <row r="241" ht="15" customHeight="1" s="1">
       <c r="A241" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>ALEXANDER MARTÍNEZ  VIDAL</t>
+          <t>NESTOR ERITH HERNÁNDEZ  MENA</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -7455,24 +7455,24 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
     <row r="242" ht="15" customHeight="1" s="1">
       <c r="A242" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>ALFREDO RODRÍGUEZ  LEÓN</t>
+          <t>LUIS ROBERTO ALMAGUER  SOLIS</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -7494,12 +7494,12 @@
     <row r="243" ht="15" customHeight="1" s="1">
       <c r="A243" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>GRISEL ORTEGA  ALVAREZ</t>
+          <t>LIDISMIR DOROTEA VEGA  ARENA</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -7521,22 +7521,22 @@
     <row r="244" ht="15" customHeight="1" s="1">
       <c r="A244" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>LEYANNE MEDINA  SANABIA</t>
+          <t>PEDRO RAFAEL ALDANA ZAPATA</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
@@ -7548,12 +7548,12 @@
     <row r="245" ht="15" customHeight="1" s="1">
       <c r="A245" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>YOELKIS VIAMONTE  MENDOZA</t>
+          <t>RACIEL PEREDA AGUILERA</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -7575,12 +7575,12 @@
     <row r="246" ht="15" customHeight="1" s="1">
       <c r="A246" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>ARIAN HECHAVARRIA CASTILLO</t>
+          <t>ANNIER  CHAVEZ  LECTO</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -7602,17 +7602,17 @@
     <row r="247" ht="15" customHeight="1" s="1">
       <c r="A247" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>ONIS GORGUET NUÑEZ</t>
+          <t>YOSVANY PRIETO  MERIÑO</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -7629,12 +7629,12 @@
     <row r="248" ht="15" customHeight="1" s="1">
       <c r="A248" t="inlineStr">
         <is>
-          <t>GRUPO DE SEGURIDAD INTERNA</t>
+          <t>DEPARTAMENTO HOLGUIN</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>ROBERTO SUÁREZ  ANTÚNEZ</t>
+          <t>CARLOS COBIRLLA AGUILERA</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -7644,24 +7644,24 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
     </row>
     <row r="249" ht="15" customHeight="1" s="1">
       <c r="A249" t="inlineStr">
         <is>
-          <t>SUBDIRECCION COMERCIAL</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>JANETT ADRIANA VÁZQUEZ  FANEGO</t>
+          <t>ILIAT REVILLA  BARRIENTOS</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -7683,12 +7683,12 @@
     <row r="250" ht="15" customHeight="1" s="1">
       <c r="A250" t="inlineStr">
         <is>
-          <t>GRUPO ALMACEN SIBONEY</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>ROLANDO RODRIGUEZ GONZALEZ</t>
+          <t>DIUNEIKY GIRÓN  NOA</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -7710,12 +7710,12 @@
     <row r="251" ht="15" customHeight="1" s="1">
       <c r="A251" t="inlineStr">
         <is>
-          <t>SUBDIRECCION DE OPERACIONES</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>ALEXEI BERNIS VILTRES</t>
+          <t>GRISEL ORTEGA  ALVAREZ</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -7725,24 +7725,24 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="252" ht="15" customHeight="1" s="1">
       <c r="A252" t="inlineStr">
         <is>
-          <t>GRUPO TALLER BOYEROS</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>ANGEL DANIEL PASCUAL  VALDÉS</t>
+          <t>LEYANNE MEDINA  SANABIA</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -7764,39 +7764,39 @@
     <row r="253" ht="15" customHeight="1" s="1">
       <c r="A253" t="inlineStr">
         <is>
-          <t>GRUPO TALLER BOYEROS</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>JOAQUIN MODESTO PERDOMO PEREZ</t>
+          <t>YOELKIS VIAMONTE  MENDOZA</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
     <row r="254" ht="15" customHeight="1" s="1">
       <c r="A254" t="inlineStr">
         <is>
-          <t>GRUPO TALLER SIBONEY</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>YOESLAN  VALDES SANCHEZ</t>
+          <t>ARIAN HECHAVARRIA CASTILLO</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -7818,17 +7818,17 @@
     <row r="255" ht="15" customHeight="1" s="1">
       <c r="A255" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>BÁRBARO PABLO GONZÁLEZ  RODRÍGUEZ</t>
+          <t>ONIS GORGUET NUÑEZ</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -7845,12 +7845,12 @@
     <row r="256" ht="15" customHeight="1" s="1">
       <c r="A256" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO AEROPUERTO</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>MARIA DEL  CARMEN CASTAÑER  AVERHOFF</t>
+          <t>ALFREDO RODRÍGUEZ  LEÓN</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -7872,12 +7872,12 @@
     <row r="257" ht="15" customHeight="1" s="1">
       <c r="A257" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIUDAD</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>LOYSLI REINALDO CORDERO GÓMEZ</t>
+          <t>JOSE ALAIN MASSO  ALMENARES</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -7899,22 +7899,22 @@
     <row r="258" ht="15" customHeight="1" s="1">
       <c r="A258" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO VARADERO</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>JOSE FRANCISCO DUQUESNE BAEZ</t>
+          <t>ARNULFO EDGAR LUNA  MENDOZA</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -7926,12 +7926,12 @@
     <row r="259" ht="15" customHeight="1" s="1">
       <c r="A259" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIENFUEGOS</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>LUIS ANGEL YERA PEREZ</t>
+          <t>ALEXANDER MARTÍNEZ  VIDAL</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -7953,17 +7953,17 @@
     <row r="260" ht="15" customHeight="1" s="1">
       <c r="A260" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO CIEGO DE AVILA</t>
+          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>EMILIO  VIÑALES  FIGUEROA</t>
+          <t>ALFREDO IGARZA  BARRIEL</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -7980,12 +7980,12 @@
     <row r="261" ht="15" customHeight="1" s="1">
       <c r="A261" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO SANTIAGO DE CUBA</t>
+          <t>GRUPO DE SEGURIDAD INTERNA</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>ILIAT REVILLA  BARRIENTOS</t>
+          <t>ROBERTO SUÁREZ  ANTÚNEZ</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -8012,7 +8012,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>GERARDO  FERNÁNDEZ BORROTO</t>
+          <t>HECTOR DANIEL MENDOZA VAZQUEZ</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -8039,7 +8039,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>EDUARDO LEYVA SIANKA</t>
+          <t>FRANCISCO JIMÉNEZ  FÚ</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -8066,7 +8066,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>ANDY  FERNANDEZ RAMON</t>
+          <t xml:space="preserve">DAYLON  QUESADA  HECHAVARRÍA </t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -8076,12 +8076,12 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t xml:space="preserve">B </t>
+          <t xml:space="preserve">R </t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t xml:space="preserve">R </t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>
@@ -8093,7 +8093,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>HECTOR DANIEL MENDOZA VAZQUEZ</t>
+          <t>ROLANDO  GONZALEZ PADRO</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -8120,7 +8120,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>ROLANDO  GONZALEZ PADRO</t>
+          <t>GERARDO  FERNÁNDEZ BORROTO</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -8147,7 +8147,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>FRANCISCO JIMÉNEZ  FÚ</t>
+          <t>EDUARDO LEYVA SIANKA</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -8174,7 +8174,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t xml:space="preserve">DAYLON  QUESADA  HECHAVARRÍA </t>
+          <t>ANDY  FERNANDEZ RAMON</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -8184,12 +8184,12 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
+          <t xml:space="preserve">B </t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
           <t xml:space="preserve">R </t>
-        </is>
-      </c>
-      <c r="E268" t="inlineStr">
-        <is>
-          <t xml:space="preserve">B </t>
         </is>
       </c>
     </row>

</xml_diff>